<commit_message>
Moved files to appropriate directories
</commit_message>
<xml_diff>
--- a/Variable List.xlsx
+++ b/Variable List.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/bfieguth_uoguelph_ca/Documents/NASEM Model Python/NASEM-Model-Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braeden\OneDrive - University of Guelph\NASEM Model Python\NASEM-Model-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1138" documentId="8_{E73D8FC5-FE87-461C-B545-8808632FB5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EBFA56A-237B-4BE1-A1BD-E6CF24B0743C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07BEF26-0260-4C3F-A6F2-330520F2031B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2205" windowWidth="29040" windowHeight="15840" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
+    <workbookView xWindow="28680" yWindow="2205" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="Input Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="347">
   <si>
     <t>Variable Name</t>
   </si>
@@ -933,13 +934,157 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Use_DNDF_IV</t>
+  </si>
+  <si>
+    <t>Select one of three NDF digestability estimates, Lg based is default</t>
+  </si>
+  <si>
+    <t>DMI_pred</t>
+  </si>
+  <si>
+    <t>Toggle DMI prediction, 0 is DMI prediction, 1 is user entered DMI</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>An_Parity_rl</t>
+  </si>
+  <si>
+    <t>Value from 1-2 representing % of multiparous cows, 2 = 100% multiparous</t>
+  </si>
+  <si>
+    <t>Trg_MilkProd</t>
+  </si>
+  <si>
+    <t>An_BW</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%DM </t>
+  </si>
+  <si>
+    <t>kg/d</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Animal bodyweight</t>
+  </si>
+  <si>
+    <t>Model requires feedstuffs and their %DM of diet</t>
+  </si>
+  <si>
+    <t>An_BCS</t>
+  </si>
+  <si>
+    <t>Body condition score, 1-5 scale</t>
+  </si>
+  <si>
+    <t>An_LactDay</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Day of lactation</t>
+  </si>
+  <si>
+    <t>Trg_MilkFatp</t>
+  </si>
+  <si>
+    <t>% milk</t>
+  </si>
+  <si>
+    <t>Target milk fat %</t>
+  </si>
+  <si>
+    <t>Target milk production</t>
+  </si>
+  <si>
+    <t>Trg_MilkTPp</t>
+  </si>
+  <si>
+    <t>Target milk protein %</t>
+  </si>
+  <si>
+    <t>Trg_MilkLacp</t>
+  </si>
+  <si>
+    <t>Target milk lactose %</t>
+  </si>
+  <si>
+    <t>DMI</t>
+  </si>
+  <si>
+    <t>An_BW_mature</t>
+  </si>
+  <si>
+    <t>Dry matter intake, user entered or predicted based on DMI_pred</t>
+  </si>
+  <si>
+    <t>Trg_FrmGain</t>
+  </si>
+  <si>
+    <t>Mature liveweight, default is 700kg</t>
+  </si>
+  <si>
+    <t>kg fresh wt/d</t>
+  </si>
+  <si>
+    <t>Target gain in body frame weight</t>
+  </si>
+  <si>
+    <t>An_GestDay</t>
+  </si>
+  <si>
+    <t>Day of gestation</t>
+  </si>
+  <si>
+    <t>An_GestLength</t>
+  </si>
+  <si>
+    <t>Typical length of gestation, default 283 days</t>
+  </si>
+  <si>
+    <t>Trg_RsrvGain</t>
+  </si>
+  <si>
+    <t>Target gain or loss of body reserves</t>
+  </si>
+  <si>
+    <t>Fet_BWbrth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calf birth weight, default is 44.1 kg </t>
+  </si>
+  <si>
+    <t>An_AgeDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal age </t>
+  </si>
+  <si>
+    <t>An_305RHA_MlkTP</t>
+  </si>
+  <si>
+    <t>kg milk TP over 305 days, Scalar to adjust the maximum milk protein response to EAA, 280kg/305d= no adjustment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,6 +1118,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1000,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1012,29 +1164,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1089,6 +1224,24 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1103,16 +1256,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14810AF2-61B0-4603-A46D-B5938E6451B2}" name="Table1" displayName="Table1" ref="A1:G1048567" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14810AF2-61B0-4603-A46D-B5938E6451B2}" name="Table1" displayName="Table1" ref="A1:G1048567" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:G1048567" xr:uid="{14810AF2-61B0-4603-A46D-B5938E6451B2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A1386A59-7380-4ABF-A70E-136A4A66DF19}" name="Order"/>
-    <tableColumn id="2" xr3:uid="{E6FEDDF7-C156-453B-92C5-3511ADFB90E7}" name="Variable Name" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{B77F9B81-0D9C-4539-9435-39A18A1A90B0}" name="Function Calculating" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E6FEDDF7-C156-453B-92C5-3511ADFB90E7}" name="Variable Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B77F9B81-0D9C-4539-9435-39A18A1A90B0}" name="Function Calculating" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{96FD868E-21E2-4C0E-98A6-67312D5FC661}" name="Returned"/>
     <tableColumn id="5" xr3:uid="{FA372AC3-A698-4C99-AC62-6845E091538D}" name="Line #"/>
-    <tableColumn id="6" xr3:uid="{BBDD159D-5AC2-4CC3-A2F1-CC758E36B6BC}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BBDD159D-5AC2-4CC3-A2F1-CC758E36B6BC}" name="Notes" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{C90E62BE-5D23-4B48-B77A-26A1A74FA141}" name="Duplicate Values"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B4C59711-313F-4930-B87F-432F2876F0BC}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{A4544BC0-902D-47F2-AB54-0B1C12C8AD1C}" name="Units"/>
+    <tableColumn id="3" xr3:uid="{789B5387-DACB-4941-AEF7-B06615230A22}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1417,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CBC222-87FC-4995-A1F1-81937BD3329A}">
   <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1600,7 @@
       <c r="A1" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1470,9 +1635,6 @@
       <c r="E2">
         <v>2886</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1490,9 +1652,6 @@
       <c r="E3">
         <v>386</v>
       </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1513,9 +1672,6 @@
       <c r="F4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1536,9 +1692,6 @@
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1559,9 +1712,6 @@
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1582,9 +1732,6 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1605,9 +1752,6 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1628,9 +1772,6 @@
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1651,9 +1792,6 @@
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1674,9 +1812,6 @@
       <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1697,9 +1832,6 @@
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1720,9 +1852,6 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1743,9 +1872,6 @@
       <c r="F14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1766,9 +1892,6 @@
       <c r="F15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1789,9 +1912,6 @@
       <c r="F16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G16" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1812,9 +1932,6 @@
       <c r="F17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G17" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1835,9 +1952,6 @@
       <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1858,9 +1972,6 @@
       <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G19" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1881,9 +1992,6 @@
       <c r="F20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1904,9 +2012,6 @@
       <c r="F21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1927,9 +2032,6 @@
       <c r="F22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1950,9 +2052,6 @@
       <c r="F23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1973,9 +2072,6 @@
       <c r="F24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1996,9 +2092,6 @@
       <c r="F25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2019,9 +2112,6 @@
       <c r="F26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2063,9 +2153,6 @@
       <c r="E28">
         <v>245</v>
       </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -2083,9 +2170,6 @@
       <c r="E29" t="s">
         <v>57</v>
       </c>
-      <c r="G29" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -2106,9 +2190,6 @@
       <c r="F30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2126,9 +2207,6 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-      <c r="G31" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -2146,11 +2224,8 @@
       <c r="E32" t="s">
         <v>7</v>
       </c>
-      <c r="G32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2166,11 +2241,8 @@
       <c r="E33" t="s">
         <v>7</v>
       </c>
-      <c r="G33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2186,11 +2258,8 @@
       <c r="E34" t="s">
         <v>65</v>
       </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2206,11 +2275,8 @@
       <c r="E35" t="s">
         <v>7</v>
       </c>
-      <c r="G35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2226,11 +2292,8 @@
       <c r="E36" t="s">
         <v>7</v>
       </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2246,11 +2309,8 @@
       <c r="E37">
         <v>458</v>
       </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2266,11 +2326,8 @@
       <c r="E38">
         <v>468</v>
       </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2286,11 +2343,8 @@
       <c r="E39">
         <v>1007</v>
       </c>
-      <c r="G39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2306,11 +2360,8 @@
       <c r="E40">
         <v>1010</v>
       </c>
-      <c r="G40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2329,12 +2380,8 @@
       <c r="F41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G41" t="str">
-        <f>B7</f>
-        <v>Fd_CP_kg/d</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2350,11 +2397,8 @@
       <c r="E42" t="s">
         <v>7</v>
       </c>
-      <c r="G42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2370,11 +2414,8 @@
       <c r="E43" t="s">
         <v>7</v>
       </c>
-      <c r="G43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2390,11 +2431,8 @@
       <c r="E44" t="s">
         <v>7</v>
       </c>
-      <c r="G44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2410,11 +2448,8 @@
       <c r="E45">
         <v>446</v>
       </c>
-      <c r="G45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2430,11 +2465,8 @@
       <c r="E46" t="s">
         <v>79</v>
       </c>
-      <c r="G46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2450,11 +2482,8 @@
       <c r="E47" t="s">
         <v>7</v>
       </c>
-      <c r="G47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2469,9 +2498,6 @@
       </c>
       <c r="E48" t="s">
         <v>82</v>
-      </c>
-      <c r="G48" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2490,9 +2516,6 @@
       <c r="E49" t="s">
         <v>7</v>
       </c>
-      <c r="G49" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -2510,9 +2533,6 @@
       <c r="E50" t="s">
         <v>85</v>
       </c>
-      <c r="G50" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
@@ -2530,9 +2550,6 @@
       <c r="E51">
         <v>1259</v>
       </c>
-      <c r="G51" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -2550,9 +2567,6 @@
       <c r="E52">
         <v>447</v>
       </c>
-      <c r="G52" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -2570,9 +2584,6 @@
       <c r="E53">
         <v>485</v>
       </c>
-      <c r="G53" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -2590,9 +2601,6 @@
       <c r="E54" t="s">
         <v>7</v>
       </c>
-      <c r="G54" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -2610,9 +2618,6 @@
       <c r="E55" t="s">
         <v>7</v>
       </c>
-      <c r="G55" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -2630,9 +2635,6 @@
       <c r="E56" t="s">
         <v>7</v>
       </c>
-      <c r="G56" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -2650,9 +2652,6 @@
       <c r="E57">
         <v>1262</v>
       </c>
-      <c r="G57" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2670,9 +2669,6 @@
       <c r="E58">
         <v>1268</v>
       </c>
-      <c r="G58" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2689,9 +2685,6 @@
       </c>
       <c r="E59">
         <v>1101</v>
-      </c>
-      <c r="G59" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5748,4 +5741,258 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FF422-2362-464E-8AF6-B12F418D3E4F}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>320</v>
+      </c>
+      <c r="B10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" t="s">
+        <v>321</v>
+      </c>
+      <c r="C11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C18" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B19" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B20" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B21" t="s">
+        <v>312</v>
+      </c>
+      <c r="C21" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>